<commit_message>
Test : OnlyPositionsTest Feature : DATAUtilities Progress
</commit_message>
<xml_diff>
--- a/src/test/resources/naukariVisualsData/NaukariVisualsData.xlsx
+++ b/src/test/resources/naukariVisualsData/NaukariVisualsData.xlsx
@@ -5,14 +5,15 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mayur Deore\IdeaProjects\ResearchAnalyst\src\test\resources\NaukariVisualsData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mayur Deore\IdeaProjects\ResearchAnalyst\src\test\resources\naukariVisualsData\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8688"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8688" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Test1" sheetId="1" r:id="rId1"/>
+    <sheet name="Testcases" sheetId="1" r:id="rId1"/>
+    <sheet name="Data" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -21,6 +22,80 @@
     </ext>
   </extLst>
 </workbook>
+</file>
+
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="23">
+  <si>
+    <t>TestCase</t>
+  </si>
+  <si>
+    <t>Runmode</t>
+  </si>
+  <si>
+    <t>LoginTest</t>
+  </si>
+  <si>
+    <t>Y</t>
+  </si>
+  <si>
+    <t>Browser</t>
+  </si>
+  <si>
+    <t>Chrome</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>Designation</t>
+  </si>
+  <si>
+    <t>Experience</t>
+  </si>
+  <si>
+    <t>Location</t>
+  </si>
+  <si>
+    <t>Test Engineer</t>
+  </si>
+  <si>
+    <t>Test Manager</t>
+  </si>
+  <si>
+    <t>Software Tester</t>
+  </si>
+  <si>
+    <t>Software test Engineer</t>
+  </si>
+  <si>
+    <t>QA Engineer</t>
+  </si>
+  <si>
+    <t>QA Tester</t>
+  </si>
+  <si>
+    <t>QA Lead</t>
+  </si>
+  <si>
+    <t>Test Specialist</t>
+  </si>
+  <si>
+    <t>Software QA Automation Engineer</t>
+  </si>
+  <si>
+    <t>Automation Engineer</t>
+  </si>
+  <si>
+    <t>Automation Tester</t>
+  </si>
+  <si>
+    <t>OnlyPositions</t>
+  </si>
+  <si>
+    <t>Total Jobs</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -34,15 +109,27 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC00000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -50,12 +137,33 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -336,14 +444,250 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="16.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.77734375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F13"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="16.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.77734375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="29.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.5546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.77734375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.44140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.5546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A1" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A2" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A3" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" s="2"/>
+      <c r="E3" s="2"/>
+      <c r="F3" s="2"/>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A4" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D4" s="2"/>
+      <c r="E4" s="2"/>
+      <c r="F4" s="2"/>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A5" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D5" s="2"/>
+      <c r="E5" s="2"/>
+      <c r="F5" s="2"/>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A6" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D6" s="2"/>
+      <c r="E6" s="2"/>
+      <c r="F6" s="2"/>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A7" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D7" s="2"/>
+      <c r="E7" s="2"/>
+      <c r="F7" s="2"/>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A8" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D8" s="2"/>
+      <c r="E8" s="2"/>
+      <c r="F8" s="2"/>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A9" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D9" s="2"/>
+      <c r="E9" s="2"/>
+      <c r="F9" s="2"/>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A10" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D10" s="2"/>
+      <c r="E10" s="2"/>
+      <c r="F10" s="2"/>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A11" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D11" s="2"/>
+      <c r="E11" s="2"/>
+      <c r="F11" s="2"/>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A12" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D12" s="2"/>
+      <c r="E12" s="2"/>
+      <c r="F12" s="2"/>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A13" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="D13" s="2"/>
+      <c r="E13" s="2"/>
+      <c r="F13" s="2"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Project: Naukari Visuals Bucket: Testing Script: OnlyPositionsTest Test Status: Completed Feature: Set Data Methods Feature Status: set data methods created in DataUtil and MyXLSReader
</commit_message>
<xml_diff>
--- a/src/test/resources/naukariVisualsData/NaukariVisualsData.xlsx
+++ b/src/test/resources/naukariVisualsData/NaukariVisualsData.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="153222"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mayur Deore\IdeaProjects\ResearchAnalyst\src\test\resources\naukariVisualsData\"/>
     </mc:Choice>
@@ -17,7 +17,7 @@
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="33">
   <si>
     <t>TestCase</t>
   </si>
@@ -45,9 +45,6 @@
     <t>Chrome</t>
   </si>
   <si>
-    <t>N</t>
-  </si>
-  <si>
     <t>Designation</t>
   </si>
   <si>
@@ -94,12 +91,46 @@
   </si>
   <si>
     <t>Total Jobs</t>
+  </si>
+  <si>
+    <t>4065</t>
+  </si>
+  <si>
+    <t>638</t>
+  </si>
+  <si>
+    <t>100192</t>
+  </si>
+  <si>
+    <t>24498</t>
+  </si>
+  <si>
+    <t>2887</t>
+  </si>
+  <si>
+    <t>11697</t>
+  </si>
+  <si>
+    <t>2531</t>
+  </si>
+  <si>
+    <t>1932</t>
+  </si>
+  <si>
+    <t>309</t>
+  </si>
+  <si>
+    <t>2776</t>
+  </si>
+  <si>
+    <t>7196</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="0"/>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -156,7 +187,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -164,6 +195,45 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="1" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment wrapText="true"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -447,13 +517,13 @@
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection sqref="A1:B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="16.88671875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.77734375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="16.88671875" collapsed="false"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="8.77734375" collapsed="false"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
@@ -474,7 +544,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>3</v>
@@ -491,25 +561,25 @@
   <dimension ref="A1:F13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="16.88671875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.77734375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="29.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.5546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.77734375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="15.44140625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="16.88671875" collapsed="false"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="7.77734375" collapsed="false"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="29.33203125" collapsed="false"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="11.0" collapsed="false"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="13.5546875" collapsed="false"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" style="6" width="9.9375" collapsed="false"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="8.77734375" collapsed="false"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="15.44140625" collapsed="false"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" width="13.5546875" collapsed="false"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
@@ -520,16 +590,16 @@
         <v>4</v>
       </c>
       <c r="C2" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="E2" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="E2" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="F2" s="4" t="s">
-        <v>22</v>
+      <c r="F2" s="7" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
@@ -540,151 +610,173 @@
         <v>5</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D3" s="2"/>
       <c r="E3" s="2"/>
-      <c r="F3" s="2"/>
+      <c r="F3" s="9" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D4" s="2"/>
       <c r="E4" s="2"/>
-      <c r="F4" s="2"/>
+      <c r="F4" s="10" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D5" s="2"/>
       <c r="E5" s="2"/>
-      <c r="F5" s="2"/>
+      <c r="F5" s="11" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D6" s="2"/>
       <c r="E6" s="2"/>
-      <c r="F6" s="2"/>
+      <c r="F6" s="12" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D7" s="2"/>
       <c r="E7" s="2"/>
-      <c r="F7" s="2"/>
+      <c r="F7" s="13" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D8" s="2"/>
       <c r="E8" s="2"/>
-      <c r="F8" s="2"/>
+      <c r="F8" s="14" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="B9" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D9" s="2"/>
       <c r="E9" s="2"/>
-      <c r="F9" s="2"/>
+      <c r="F9" s="15" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="B10" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D10" s="2"/>
       <c r="E10" s="2"/>
-      <c r="F10" s="2"/>
+      <c r="F10" s="16" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="B11" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D11" s="2"/>
       <c r="E11" s="2"/>
-      <c r="F11" s="2"/>
+      <c r="F11" s="17" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="B12" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D12" s="2"/>
       <c r="E12" s="2"/>
-      <c r="F12" s="2"/>
+      <c r="F12" s="18" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="B13" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D13" s="2"/>
       <c r="E13" s="2"/>
-      <c r="F13" s="2"/>
+      <c r="F13" s="19" t="s">
+        <v>32</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Project: Naukari Visuals Bucket: Testing Script: Skills Test Status: Completed
</commit_message>
<xml_diff>
--- a/src/test/resources/naukariVisualsData/NaukariVisualsData.xlsx
+++ b/src/test/resources/naukariVisualsData/NaukariVisualsData.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="58">
   <si>
     <t>TestCase</t>
   </si>
@@ -93,37 +93,112 @@
     <t>Total Jobs</t>
   </si>
   <si>
-    <t>4065</t>
-  </si>
-  <si>
-    <t>638</t>
-  </si>
-  <si>
-    <t>100192</t>
-  </si>
-  <si>
-    <t>24498</t>
-  </si>
-  <si>
-    <t>2887</t>
-  </si>
-  <si>
-    <t>11697</t>
-  </si>
-  <si>
-    <t>2531</t>
-  </si>
-  <si>
-    <t>1932</t>
-  </si>
-  <si>
-    <t>309</t>
-  </si>
-  <si>
-    <t>2776</t>
-  </si>
-  <si>
-    <t>7196</t>
+    <t>4076</t>
+  </si>
+  <si>
+    <t>639</t>
+  </si>
+  <si>
+    <t>100315</t>
+  </si>
+  <si>
+    <t>24546</t>
+  </si>
+  <si>
+    <t>2886</t>
+  </si>
+  <si>
+    <t>11702</t>
+  </si>
+  <si>
+    <t>2530</t>
+  </si>
+  <si>
+    <t>1938</t>
+  </si>
+  <si>
+    <t>311</t>
+  </si>
+  <si>
+    <t>2781</t>
+  </si>
+  <si>
+    <t>7197</t>
+  </si>
+  <si>
+    <t>Skills</t>
+  </si>
+  <si>
+    <t>Selenium</t>
+  </si>
+  <si>
+    <t>Cypress</t>
+  </si>
+  <si>
+    <t>Cucumber</t>
+  </si>
+  <si>
+    <t>Apache JMeter</t>
+  </si>
+  <si>
+    <t>Katalon</t>
+  </si>
+  <si>
+    <t>Appium</t>
+  </si>
+  <si>
+    <t>Tricentis Tosca</t>
+  </si>
+  <si>
+    <t>LambdaTest</t>
+  </si>
+  <si>
+    <t>TestRail</t>
+  </si>
+  <si>
+    <t>BrowserStack</t>
+  </si>
+  <si>
+    <t>Zephyr</t>
+  </si>
+  <si>
+    <t>QTP</t>
+  </si>
+  <si>
+    <t>8838</t>
+  </si>
+  <si>
+    <t>5080</t>
+  </si>
+  <si>
+    <t>1803</t>
+  </si>
+  <si>
+    <t>3705</t>
+  </si>
+  <si>
+    <t>253</t>
+  </si>
+  <si>
+    <t>1246</t>
+  </si>
+  <si>
+    <t>33</t>
+  </si>
+  <si>
+    <t>17</t>
+  </si>
+  <si>
+    <t>196</t>
+  </si>
+  <si>
+    <t>104</t>
+  </si>
+  <si>
+    <t>247</t>
+  </si>
+  <si>
+    <t>6959</t>
   </si>
 </sst>
 </file>
@@ -187,7 +262,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -195,12 +270,44 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment wrapText="true"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment wrapText="true"/>
     </xf>
@@ -514,16 +621,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:B3"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="16.88671875" collapsed="false"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="8.77734375" collapsed="false"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="16.88671875" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="8.77734375" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
@@ -547,6 +654,14 @@
         <v>20</v>
       </c>
       <c r="B3" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B4" s="2" t="s">
         <v>3</v>
       </c>
     </row>
@@ -558,23 +673,23 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F13"/>
+  <dimension ref="A1:I28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+      <selection activeCell="J24" sqref="J24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="16.88671875" collapsed="false"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="7.77734375" collapsed="false"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="29.33203125" collapsed="false"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="11.0" collapsed="false"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="13.5546875" collapsed="false"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" style="6" width="9.9375" collapsed="false"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" width="8.77734375" collapsed="false"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" width="15.44140625" collapsed="false"/>
-    <col min="9" max="9" bestFit="true" customWidth="true" width="13.5546875" collapsed="false"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="16.88671875" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="7.77734375" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="29.33203125" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="11.0" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="13.5546875" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" style="5" width="9.9375" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="8.77734375" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="15.44140625" collapsed="true"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" width="13.5546875" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.3">
@@ -598,7 +713,7 @@
       <c r="E2" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="F2" s="7" t="s">
+      <c r="F2" s="6" t="s">
         <v>21</v>
       </c>
     </row>
@@ -614,7 +729,7 @@
       </c>
       <c r="D3" s="2"/>
       <c r="E3" s="2"/>
-      <c r="F3" s="9" t="s">
+      <c r="F3" s="7" t="s">
         <v>22</v>
       </c>
     </row>
@@ -630,7 +745,7 @@
       </c>
       <c r="D4" s="2"/>
       <c r="E4" s="2"/>
-      <c r="F4" s="10" t="s">
+      <c r="F4" s="8" t="s">
         <v>23</v>
       </c>
     </row>
@@ -646,7 +761,7 @@
       </c>
       <c r="D5" s="2"/>
       <c r="E5" s="2"/>
-      <c r="F5" s="11" t="s">
+      <c r="F5" s="9" t="s">
         <v>24</v>
       </c>
     </row>
@@ -662,7 +777,7 @@
       </c>
       <c r="D6" s="2"/>
       <c r="E6" s="2"/>
-      <c r="F6" s="12" t="s">
+      <c r="F6" s="10" t="s">
         <v>25</v>
       </c>
     </row>
@@ -678,7 +793,7 @@
       </c>
       <c r="D7" s="2"/>
       <c r="E7" s="2"/>
-      <c r="F7" s="13" t="s">
+      <c r="F7" s="11" t="s">
         <v>26</v>
       </c>
     </row>
@@ -694,7 +809,7 @@
       </c>
       <c r="D8" s="2"/>
       <c r="E8" s="2"/>
-      <c r="F8" s="14" t="s">
+      <c r="F8" s="12" t="s">
         <v>27</v>
       </c>
     </row>
@@ -710,7 +825,7 @@
       </c>
       <c r="D9" s="2"/>
       <c r="E9" s="2"/>
-      <c r="F9" s="15" t="s">
+      <c r="F9" s="13" t="s">
         <v>28</v>
       </c>
     </row>
@@ -726,7 +841,7 @@
       </c>
       <c r="D10" s="2"/>
       <c r="E10" s="2"/>
-      <c r="F10" s="16" t="s">
+      <c r="F10" s="14" t="s">
         <v>29</v>
       </c>
     </row>
@@ -742,7 +857,7 @@
       </c>
       <c r="D11" s="2"/>
       <c r="E11" s="2"/>
-      <c r="F11" s="17" t="s">
+      <c r="F11" s="15" t="s">
         <v>30</v>
       </c>
     </row>
@@ -758,7 +873,7 @@
       </c>
       <c r="D12" s="2"/>
       <c r="E12" s="2"/>
-      <c r="F12" s="18" t="s">
+      <c r="F12" s="16" t="s">
         <v>31</v>
       </c>
     </row>
@@ -774,12 +889,236 @@
       </c>
       <c r="D13" s="2"/>
       <c r="E13" s="2"/>
-      <c r="F13" s="19" t="s">
+      <c r="F13" s="17" t="s">
         <v>32</v>
       </c>
     </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A15" s="3" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A16" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B16" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D16" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E16" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="F16" s="6" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A17" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="D17" s="2"/>
+      <c r="E17" s="2"/>
+      <c r="F17" s="18" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A18" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="D18" s="2"/>
+      <c r="E18" s="2"/>
+      <c r="F18" s="19" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A19" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="D19" s="2"/>
+      <c r="E19" s="2"/>
+      <c r="F19" s="20" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A20" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="D20" s="2"/>
+      <c r="E20" s="2"/>
+      <c r="F20" s="21" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A21" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="D21" s="2"/>
+      <c r="E21" s="2"/>
+      <c r="F21" s="22" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A22" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="D22" s="2"/>
+      <c r="E22" s="2"/>
+      <c r="F22" s="23" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A23" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="D23" s="2"/>
+      <c r="E23" s="2"/>
+      <c r="F23" s="24" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A24" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="D24" s="2"/>
+      <c r="E24" s="2"/>
+      <c r="F24" s="25" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A25" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="D25" s="2"/>
+      <c r="E25" s="2"/>
+      <c r="F25" s="26" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A26" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="D26" s="2"/>
+      <c r="E26" s="2"/>
+      <c r="F26" s="27" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A27" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C27" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="D27" s="2"/>
+      <c r="E27" s="2"/>
+      <c r="F27" s="28" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A28" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C28" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="D28" s="2"/>
+      <c r="E28" s="2"/>
+      <c r="F28" s="29" t="s">
+        <v>57</v>
+      </c>
+    </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C23" r:id="rId1" display="https://www.google.com/search?rlz=1C1UEAD_enIN977IN977&amp;cs=1&amp;sxsrf=APwXEdeaap-FvmAl6QuswwbFY2iv6WmoBg:1686504200947&amp;q=tricentis+tosca&amp;stick=H4sIAAAAAAAAAOMwVGIyNIviLUktLsnMS1coyc_PKf7FyBuCwmfiiHf1C_EMiYzfwML4ioWbi1M_V98g2cLIouwVCw8XF4hnUplWYJ70ioWfi1c_Xd_QMN0gPaWssqACIZJsamliWFRlCDfApLIgOQNugJF5jrFFClwypdC4Kg0uaZxiUZxWAJfMMLSojIdLJptUGVoADVKEcFPSc6vSLISEQ1JzUosysxVAflEILilNycyHG2CeZ5iXgnBaUnmeaUFxQTrcyOLy7MKsKoSCDOOcLPOkyhIkLcmmyQY5ueVIPjaLTy6IrzRAUpNUUVhlUWz8ioWXixtkrKFRkWGVee4rFi4uDjA_PaMSEZ7ZGTmI8My2tMjJKHrFwsfFAzLLyLSkxCjdBBgEXEIcIB8FJWbmLGLlLynKTE7NK8ksBkZVcXLiLTZJhpJn12Z1rG47uv0UX-2xeQuDxK4EVlwQnDMVAIQJ69bsAQAA&amp;sa=X&amp;ved=2ahUKEwiRjrze3bv_AhUgTGwGHa0zBm0Q7fAIegUIABCwAQ"/>
+    <hyperlink ref="C27" r:id="rId2" display="https://guru99.link/4h5dh2"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId3"/>
+  <ignoredErrors>
+    <ignoredError sqref="F3" numberStoredAsText="1"/>
+  </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>